<commit_message>
Updated MDI_Raven_Excel_Schema to version 1.1 with org support.
</commit_message>
<xml_diff>
--- a/MDI_Raven_Excel_Schema.xlsx
+++ b/MDI_Raven_Excel_Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273B37C2-A6AB-4E62-91C5-68817CC99A07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC6BFF82-2DF5-42E0-82F3-1BC2B8397114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="MDI RAVEN Input Schema" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="176">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -624,6 +624,47 @@
   </si>
   <si>
     <t>Black or African American</t>
+  </si>
+  <si>
+    <t>File Id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IMPORTANT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">This cell is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REQUIRED</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for the entire sheet. In order to persist records properly, you must assign an id to this sheet. It is recommended to assign this field as &lt;organization_name&gt;-&lt;id&gt;. File id's must be unique across all files. No whitespace or special characters allowed.</t>
+    </r>
+  </si>
+  <si>
+    <t>INVALID</t>
   </si>
 </sst>
 </file>
@@ -633,7 +674,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,6 +685,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -694,6 +736,13 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -817,7 +866,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -888,6 +937,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -896,7 +971,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1310,6 +1385,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1647,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="D55" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -1692,48 +1773,44 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="82" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A3" s="59" t="s">
+    <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="134" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="135" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="111" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="111" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A4" s="60"/>
-      <c r="B4" s="131" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
+      <c r="A5" s="60"/>
+      <c r="B5" s="131" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="112" t="s">
+      <c r="C5" s="112" t="s">
         <v>105</v>
-      </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A5" s="60"/>
-      <c r="B5" s="132" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="112" t="s">
-        <v>106</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="57"/>
@@ -1742,43 +1819,43 @@
       <c r="H5" s="57"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A6" s="61" t="s">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A6" s="60"/>
+      <c r="B6" s="132" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A7" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="113" t="s">
+      <c r="B7" s="75"/>
+      <c r="C7" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A7" s="62"/>
-      <c r="B7" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
       <c r="A8" s="62"/>
       <c r="B8" s="83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="114" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="9"/>
@@ -1787,13 +1864,13 @@
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A9" s="62"/>
       <c r="B9" s="83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="114" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="9"/>
@@ -1802,13 +1879,13 @@
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A10" s="62"/>
-      <c r="B10" s="84" t="s">
-        <v>78</v>
+      <c r="B10" s="83" t="s">
+        <v>12</v>
       </c>
       <c r="C10" s="114" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="9"/>
@@ -1817,13 +1894,13 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
       <c r="A11" s="62"/>
-      <c r="B11" s="83" t="s">
-        <v>13</v>
+      <c r="B11" s="84" t="s">
+        <v>78</v>
       </c>
       <c r="C11" s="114" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="9"/>
@@ -1832,13 +1909,13 @@
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A12" s="62"/>
       <c r="B12" s="83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="9"/>
@@ -1847,66 +1924,68 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
       <c r="A13" s="62"/>
       <c r="B13" s="83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="114" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="95"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A14" s="62"/>
       <c r="B14" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="114"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="C14" s="114" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="95"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="62"/>
       <c r="B15" s="83" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="114" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+        <v>16</v>
+      </c>
+      <c r="C15" s="114"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A16" s="62"/>
       <c r="B16" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="114"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="C16" s="114" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="96"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A17" s="62"/>
       <c r="B17" s="83" t="s">
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="C17" s="114"/>
       <c r="D17" s="14"/>
@@ -1916,10 +1995,10 @@
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="62"/>
-      <c r="B18" s="85" t="s">
-        <v>19</v>
+      <c r="B18" s="83" t="s">
+        <v>102</v>
       </c>
       <c r="C18" s="114"/>
       <c r="D18" s="14"/>
@@ -1929,10 +2008,10 @@
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A19" s="62"/>
-      <c r="B19" s="83" t="s">
-        <v>38</v>
+      <c r="B19" s="85" t="s">
+        <v>19</v>
       </c>
       <c r="C19" s="114"/>
       <c r="D19" s="14"/>
@@ -1945,7 +2024,7 @@
     <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A20" s="62"/>
       <c r="B20" s="83" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C20" s="114"/>
       <c r="D20" s="14"/>
@@ -1955,73 +2034,71 @@
       <c r="H20" s="9"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A21" s="127" t="s">
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="62"/>
+      <c r="B21" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="114"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A22" s="127" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="115" t="s">
+      <c r="B22" s="76"/>
+      <c r="C22" s="115" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="63"/>
-      <c r="B22" s="133" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="97"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A23" s="63"/>
       <c r="B23" s="133" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="116" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="98"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+        <v>116</v>
+      </c>
+      <c r="D23" s="97"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="63"/>
       <c r="B24" s="133" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="99"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+        <v>117</v>
+      </c>
+      <c r="D24" s="98"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A25" s="63"/>
       <c r="B25" s="133" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="C25" s="116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="99"/>
       <c r="E25" s="21"/>
@@ -2030,13 +2107,13 @@
       <c r="H25" s="21"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A26" s="63"/>
       <c r="B26" s="133" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="C26" s="116" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="99"/>
       <c r="E26" s="21"/>
@@ -2048,10 +2125,10 @@
     <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A27" s="63"/>
       <c r="B27" s="133" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" s="99"/>
       <c r="E27" s="21"/>
@@ -2063,10 +2140,10 @@
     <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A28" s="63"/>
       <c r="B28" s="133" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C28" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D28" s="99"/>
       <c r="E28" s="21"/>
@@ -2078,40 +2155,40 @@
     <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A29" s="63"/>
       <c r="B29" s="133" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="116" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="97"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
+        <v>122</v>
+      </c>
+      <c r="D29" s="99"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A30" s="63"/>
       <c r="B30" s="133" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="116" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="97"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A31" s="63"/>
+      <c r="B31" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="116" t="s">
+      <c r="C31" s="116" t="s">
         <v>124</v>
-      </c>
-      <c r="D30" s="100"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="18"/>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A31" s="63"/>
-      <c r="B31" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="116" t="s">
-        <v>125</v>
       </c>
       <c r="D31" s="100"/>
       <c r="E31" s="22"/>
@@ -2120,73 +2197,73 @@
       <c r="H31" s="22"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A32" s="63"/>
       <c r="B32" s="86" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="C32" s="116" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" s="101"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+        <v>125</v>
+      </c>
+      <c r="D32" s="100"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
       <c r="A33" s="63"/>
       <c r="B33" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="116" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="101"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A34" s="63"/>
+      <c r="B34" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C34" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="100"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="18"/>
-    </row>
-    <row r="34" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="64"/>
-      <c r="B34" s="86" t="s">
+      <c r="D34" s="100"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="64"/>
+      <c r="B35" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C35" s="116" t="s">
         <v>128</v>
       </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A35" s="63"/>
-      <c r="B35" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="100"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="18"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
       <c r="A36" s="63"/>
       <c r="B36" s="86" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" s="100"/>
       <c r="E36" s="22"/>
@@ -2195,223 +2272,223 @@
       <c r="H36" s="22"/>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A37" s="128" t="s">
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A37" s="63"/>
+      <c r="B37" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="116" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="100"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A38" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="117" t="s">
+      <c r="B38" s="77"/>
+      <c r="C38" s="117" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-    </row>
-    <row r="38" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="65"/>
-      <c r="B38" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="118" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" s="102"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="30"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A39" s="65"/>
-      <c r="B39" s="88" t="s">
-        <v>99</v>
+      <c r="B39" s="87" t="s">
+        <v>39</v>
       </c>
       <c r="C39" s="118" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="D39" s="102"/>
       <c r="E39" s="29"/>
-      <c r="F39" s="32"/>
+      <c r="F39" s="29"/>
       <c r="G39" s="29"/>
-      <c r="H39" s="32"/>
+      <c r="H39" s="29"/>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A40" s="65"/>
-      <c r="B40" s="87" t="s">
-        <v>79</v>
+      <c r="B40" s="88" t="s">
+        <v>99</v>
       </c>
       <c r="C40" s="118" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="D40" s="102"/>
-      <c r="E40" s="102"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="102"/>
-      <c r="H40" s="102"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="32"/>
       <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
       <c r="A41" s="65"/>
-      <c r="B41" s="130" t="s">
+      <c r="B41" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="102"/>
+      <c r="E41" s="102"/>
+      <c r="F41" s="102"/>
+      <c r="G41" s="102"/>
+      <c r="H41" s="102"/>
+      <c r="I41" s="30"/>
+    </row>
+    <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A42" s="65"/>
+      <c r="B42" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="118" t="s">
+      <c r="C42" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="102"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="30"/>
-    </row>
-    <row r="42" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A42" s="66" t="s">
+      <c r="D42" s="102"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="30"/>
+    </row>
+    <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A43" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="119" t="s">
+      <c r="B43" s="78"/>
+      <c r="C43" s="119" t="s">
         <v>147</v>
       </c>
-      <c r="D42" s="103"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="34"/>
-    </row>
-    <row r="43" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A43" s="67"/>
-      <c r="B43" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="120" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="104"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
-    </row>
-    <row r="44" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="D43" s="103"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="34"/>
+    </row>
+    <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A44" s="67"/>
       <c r="B44" s="89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" s="120" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" s="105"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
+        <v>134</v>
+      </c>
+      <c r="D44" s="104"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="37"/>
     </row>
-    <row r="45" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
       <c r="A45" s="67"/>
       <c r="B45" s="89" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="C45" s="120" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="106"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
+        <v>135</v>
+      </c>
+      <c r="D45" s="105"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
       <c r="I45" s="37"/>
     </row>
-    <row r="46" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
       <c r="A46" s="67"/>
       <c r="B46" s="89" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="C46" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="D46" s="107"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
+        <v>140</v>
+      </c>
+      <c r="D46" s="106"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
       <c r="I46" s="37"/>
     </row>
-    <row r="47" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
       <c r="A47" s="67"/>
       <c r="B47" s="89" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" s="120" t="s">
-        <v>142</v>
-      </c>
-      <c r="D47" s="105"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
+        <v>141</v>
+      </c>
+      <c r="D47" s="107"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
       <c r="I47" s="37"/>
     </row>
-    <row r="48" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
       <c r="A48" s="67"/>
       <c r="B48" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="120" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="105"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="37"/>
+    </row>
+    <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A49" s="67"/>
+      <c r="B49" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="120" t="s">
+      <c r="C49" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="37"/>
-    </row>
-    <row r="49" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A49" s="68" t="s">
+      <c r="D49" s="106"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="37"/>
+    </row>
+    <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A50" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="79"/>
-      <c r="C49" s="121" t="s">
+      <c r="B50" s="79"/>
+      <c r="C50" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-    </row>
-    <row r="50" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="69"/>
-      <c r="B50" s="90" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="122" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" s="108"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="45"/>
-    </row>
-    <row r="51" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+    </row>
+    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A51" s="69"/>
       <c r="B51" s="90" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C51" s="122" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D51" s="108"/>
       <c r="E51" s="44"/>
@@ -2420,43 +2497,43 @@
       <c r="H51" s="44"/>
       <c r="I51" s="45"/>
     </row>
-    <row r="52" spans="1:9" s="48" customFormat="1" ht="42" x14ac:dyDescent="0.5">
-      <c r="A52" s="129" t="s">
+    <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A52" s="69"/>
+      <c r="B52" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="122" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="108"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="45"/>
+    </row>
+    <row r="53" spans="1:9" s="48" customFormat="1" ht="42" x14ac:dyDescent="0.5">
+      <c r="A53" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="80"/>
-      <c r="C52" s="123" t="s">
+      <c r="B53" s="80"/>
+      <c r="C53" s="123" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-    </row>
-    <row r="53" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A53" s="70"/>
-      <c r="B53" s="91" t="s">
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47"/>
+    </row>
+    <row r="54" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A54" s="70"/>
+      <c r="B54" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="124" t="s">
+      <c r="C54" s="124" t="s">
         <v>150</v>
-      </c>
-      <c r="D53" s="109"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="50"/>
-    </row>
-    <row r="54" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A54" s="70"/>
-      <c r="B54" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="124" t="s">
-        <v>151</v>
       </c>
       <c r="D54" s="109"/>
       <c r="E54" s="49"/>
@@ -2465,13 +2542,13 @@
       <c r="H54" s="49"/>
       <c r="I54" s="50"/>
     </row>
-    <row r="55" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
       <c r="A55" s="70"/>
-      <c r="B55" s="91" t="s">
-        <v>94</v>
+      <c r="B55" s="92" t="s">
+        <v>93</v>
       </c>
       <c r="C55" s="124" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D55" s="109"/>
       <c r="E55" s="49"/>
@@ -2483,10 +2560,10 @@
     <row r="56" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A56" s="70"/>
       <c r="B56" s="91" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="C56" s="124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56" s="109"/>
       <c r="E56" s="49"/>
@@ -2495,12 +2572,14 @@
       <c r="H56" s="49"/>
       <c r="I56" s="50"/>
     </row>
-    <row r="57" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A57" s="70"/>
       <c r="B57" s="91" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="124"/>
+        <v>33</v>
+      </c>
+      <c r="C57" s="124" t="s">
+        <v>153</v>
+      </c>
       <c r="D57" s="109"/>
       <c r="E57" s="49"/>
       <c r="F57" s="49"/>
@@ -2511,7 +2590,7 @@
     <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A58" s="70"/>
       <c r="B58" s="91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C58" s="124"/>
       <c r="D58" s="109"/>
@@ -2521,10 +2600,10 @@
       <c r="H58" s="49"/>
       <c r="I58" s="50"/>
     </row>
-    <row r="59" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A59" s="70"/>
-      <c r="B59" s="93" t="s">
-        <v>36</v>
+      <c r="B59" s="91" t="s">
+        <v>35</v>
       </c>
       <c r="C59" s="124"/>
       <c r="D59" s="109"/>
@@ -2534,10 +2613,10 @@
       <c r="H59" s="49"/>
       <c r="I59" s="50"/>
     </row>
-    <row r="60" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
       <c r="A60" s="70"/>
       <c r="B60" s="93" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C60" s="124"/>
       <c r="D60" s="109"/>
@@ -2547,43 +2626,41 @@
       <c r="H60" s="49"/>
       <c r="I60" s="50"/>
     </row>
-    <row r="61" spans="1:9" s="53" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A61" s="71" t="s">
+    <row r="61" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A61" s="70"/>
+      <c r="B61" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="124"/>
+      <c r="D61" s="109"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="50"/>
+    </row>
+    <row r="62" spans="1:9" s="53" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A62" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="81"/>
-      <c r="C61" s="125" t="s">
+      <c r="B62" s="81"/>
+      <c r="C62" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="52"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="52"/>
-    </row>
-    <row r="62" spans="1:9" s="56" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A62" s="72"/>
-      <c r="B62" s="94" t="s">
-        <v>97</v>
-      </c>
-      <c r="C62" s="126" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" s="110"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="55"/>
-    </row>
-    <row r="63" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+    </row>
+    <row r="63" spans="1:9" s="56" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
       <c r="A63" s="72"/>
       <c r="B63" s="94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C63" s="126" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D63" s="110"/>
       <c r="E63" s="54"/>
@@ -2591,6 +2668,21 @@
       <c r="G63" s="54"/>
       <c r="H63" s="54"/>
       <c r="I63" s="55"/>
+    </row>
+    <row r="64" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="72"/>
+      <c r="B64" s="94" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="126" t="s">
+        <v>166</v>
+      </c>
+      <c r="D64" s="110"/>
+      <c r="E64" s="54"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="54"/>
+      <c r="I64" s="55"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2603,73 +2695,73 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D8</xm:sqref>
+          <xm:sqref>D9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2560A1C6-3FEA-4452-84E2-D4BC7FEE35BC}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D9:H9</xm:sqref>
+          <xm:sqref>D10:H10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6714C258-4BD2-45CC-BA09-55489A06314D}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:H10</xm:sqref>
+          <xm:sqref>D11:H11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EE5A822-FD38-4314-981B-8ED84EDD69EC}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$E$2:$E$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D31:H31</xm:sqref>
+          <xm:sqref>D32:H32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC01C7B9-BA05-42AD-B9A9-F2FD4557F0F1}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$F$2:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D35:H35</xm:sqref>
+          <xm:sqref>D36:H36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7CC0EF60-AEB4-4234-B37C-4A02B7E2DE3B}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D36:H36</xm:sqref>
+          <xm:sqref>D37:H37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D99AC123-497D-47BE-A346-1D3330E13BAC}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D41:H41</xm:sqref>
+          <xm:sqref>D42:H42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2388147A-1FAB-42AF-9190-67DEDF83A4EA}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$J$2:$J$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D48:H48</xm:sqref>
+          <xm:sqref>D49:H49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{093E1169-867D-4A32-AC3C-DC58C26E3C39}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D63:H63</xm:sqref>
+          <xm:sqref>D64:H64</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:H8</xm:sqref>
+          <xm:sqref>E9:H9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38BD6F45-E1D6-4C47-97BB-112AE837004E}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!K2:K4</xm:f>
           </x14:formula1>
-          <xm:sqref>D45:H45</xm:sqref>
+          <xm:sqref>D46:H46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$L$2:$L$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D40:H40</xm:sqref>
+          <xm:sqref>D41:H41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2681,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8BFBD-18C1-4ED5-A02E-9841686C259E}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2939,56 +3031,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -3187,7 +3229,66 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
@@ -3201,24 +3302,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3238,28 +3322,36 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Pronouncer handling. Added common services for Tox-To-MDI Importing.
</commit_message>
<xml_diff>
--- a/MDI_Raven_Excel_Schema.xlsx
+++ b/MDI_Raven_Excel_Schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC6BFF82-2DF5-42E0-82F3-1BC2B8397114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE67D22F-79E4-4C12-BCDB-447B2AE0AFDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="177">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t>Asked But Unknown</t>
-  </si>
-  <si>
-    <t>Chief Medical Examiner/Coroner</t>
   </si>
   <si>
     <t>Natural death</t>
@@ -539,9 +536,6 @@
     <t>This section describes the autopsy findings, if an autopsy occurred.</t>
   </si>
   <si>
-    <t>This section describes the primary Chief Medical Examiner or Coroner associated to the case.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of the Medical Examiner.
 Accepted Formats:
 &lt;First Name&gt; &lt;Last Name&gt;
@@ -559,9 +553,6 @@
   </si>
   <si>
     <t>Primary Address of the medical examiner's office or primary address. Multiple lines are supported.</t>
-  </si>
-  <si>
-    <t>This section describes the certifier of the case, if the case has been certified. Oftentimes, the Chief Medical Examiner and the Certifier can be the same party. If the case is not certified, leave blank</t>
   </si>
   <si>
     <t xml:space="preserve">Name of the Certifier.
@@ -664,17 +655,30 @@
     </r>
   </si>
   <si>
-    <t>INVALID</t>
+    <t>GTRI</t>
+  </si>
+  <si>
+    <t>This section describes the primary Medical Examiner or Coroner associated to the case.</t>
+  </si>
+  <si>
+    <t>This section describes the certifier of the case, if the case has been certified. Oftentimes, the Medical Examiner/Coroner and the Certifier can be the same party. If the case is not certified, leave blank</t>
+  </si>
+  <si>
+    <t>Pronouncer of death</t>
+  </si>
+  <si>
+    <t>The person who is pronouncing the place and time of death. 
+Accepted Formats:
+&lt;First Name&gt; &lt;Last Name&gt;
+&lt;First Name&gt; &lt;Middle Initial&gt; &lt;Last Name&gt;
+&lt;First Name&gt; &lt;Middle Name&gt; &lt;Last Name&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-  </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,8 +750,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -865,6 +876,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFB3"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -971,7 +994,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1001,10 +1024,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1012,18 +1031,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1031,35 +1038,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1077,10 +1060,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1088,13 +1067,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1102,10 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1113,18 +1081,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1132,10 +1088,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1150,10 +1102,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1168,19 +1116,11 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -1252,70 +1192,6 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1391,6 +1267,163 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="11" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="22" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="11" fillId="22" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="18" fontId="11" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1728,30 +1761,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="58" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="73" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="82" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="37" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="52" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="61" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="73" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="61" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1761,41 +1794,41 @@
         <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="97" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="98" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="74" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="134" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="135" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="111" t="s">
-        <v>104</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1805,884 +1838,899 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A5" s="60"/>
-      <c r="B5" s="131" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A6" s="39"/>
+      <c r="B6" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C6" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="60"/>
-      <c r="B6" s="132" t="s">
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A7" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A8" s="41"/>
+      <c r="B8" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="111"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" s="10" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A9" s="41"/>
+      <c r="B9" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="111"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" s="10" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A10" s="41"/>
+      <c r="B10" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="111"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" s="10" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A11" s="41"/>
+      <c r="B11" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="111"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" s="10" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A12" s="41"/>
+      <c r="B12" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="111"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" s="10" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A13" s="41"/>
+      <c r="B13" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="111"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" s="10" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A14" s="41"/>
+      <c r="B14" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="111"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="41"/>
+      <c r="B15" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="77"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" s="10" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A16" s="41"/>
+      <c r="B16" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="113"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="41"/>
+      <c r="B17" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="77"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="41"/>
+      <c r="B18" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="77"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A19" s="41"/>
+      <c r="B19" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="77"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="41"/>
+      <c r="B20" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="77"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="41"/>
+      <c r="B21" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="77"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" s="12" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A22" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="55"/>
+      <c r="C22" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="42"/>
+      <c r="B23" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="116"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="42"/>
+      <c r="B24" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="79" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="118"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="119"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="42"/>
+      <c r="B25" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="120"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="42"/>
+      <c r="B26" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="120"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="121"/>
+      <c r="G26" s="121"/>
+      <c r="H26" s="121"/>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A27" s="42"/>
+      <c r="B27" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="79" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="120"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="121"/>
+      <c r="G27" s="121"/>
+      <c r="H27" s="121"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A28" s="42"/>
+      <c r="B28" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="120"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A29" s="42"/>
+      <c r="B29" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="120"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
+      <c r="G29" s="121"/>
+      <c r="H29" s="121"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A30" s="42"/>
+      <c r="B30" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="116"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="117"/>
+      <c r="H30" s="117"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" s="14" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A31" s="42"/>
+      <c r="B31" s="96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="122"/>
+      <c r="E31" s="123"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="123"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" s="14" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A32" s="42"/>
+      <c r="B32" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="79" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="122"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" s="14" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A33" s="42"/>
+      <c r="B33" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="100"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="99"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" s="14" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A34" s="42"/>
+      <c r="B34" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="102"/>
+      <c r="E34" s="103"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="43"/>
+      <c r="B35" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="79" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="120"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="121"/>
+      <c r="G35" s="121"/>
+      <c r="H35" s="121"/>
+      <c r="I35" s="15"/>
+    </row>
+    <row r="36" spans="1:9" s="14" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A36" s="42"/>
+      <c r="B36" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="79" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="122"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="123"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:9" s="14" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A37" s="42"/>
+      <c r="B37" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="122"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="123"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" s="18" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A38" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="56"/>
+      <c r="C38" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" s="124"/>
+      <c r="E38" s="124"/>
+      <c r="F38" s="124"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="1:9" s="20" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A39" s="44"/>
+      <c r="B39" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="81" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="125"/>
+      <c r="E39" s="126"/>
+      <c r="F39" s="126"/>
+      <c r="G39" s="126"/>
+      <c r="H39" s="126"/>
+      <c r="I39" s="19"/>
+    </row>
+    <row r="40" spans="1:9" s="20" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A40" s="44"/>
+      <c r="B40" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="125"/>
+      <c r="E40" s="126"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="126"/>
+      <c r="H40" s="127"/>
+      <c r="I40" s="19"/>
+    </row>
+    <row r="41" spans="1:9" s="20" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A41" s="44"/>
+      <c r="B41" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="81" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="125"/>
+      <c r="E41" s="125"/>
+      <c r="F41" s="125"/>
+      <c r="G41" s="125"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="19"/>
+    </row>
+    <row r="42" spans="1:9" s="20" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A42" s="44"/>
+      <c r="B42" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="125"/>
+      <c r="E42" s="126"/>
+      <c r="F42" s="126"/>
+      <c r="G42" s="126"/>
+      <c r="H42" s="126"/>
+      <c r="I42" s="19"/>
+    </row>
+    <row r="43" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A43" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="57"/>
+      <c r="C43" s="82" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="128"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="21"/>
+    </row>
+    <row r="44" spans="1:9" s="24" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A44" s="46"/>
+      <c r="B44" s="68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="83" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="105"/>
+      <c r="E44" s="106"/>
+      <c r="F44" s="106"/>
+      <c r="G44" s="106"/>
+      <c r="H44" s="106"/>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" s="24" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A45" s="46"/>
+      <c r="B45" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="107"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="108"/>
+      <c r="I45" s="23"/>
+    </row>
+    <row r="46" spans="1:9" s="24" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A46" s="46"/>
+      <c r="B46" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="130"/>
+      <c r="E46" s="131"/>
+      <c r="F46" s="131"/>
+      <c r="G46" s="131"/>
+      <c r="H46" s="131"/>
+      <c r="I46" s="23"/>
+    </row>
+    <row r="47" spans="1:9" s="24" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A47" s="46"/>
+      <c r="B47" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="105"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="106"/>
+      <c r="G47" s="106"/>
+      <c r="H47" s="106"/>
+      <c r="I47" s="23"/>
+    </row>
+    <row r="48" spans="1:9" s="24" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+      <c r="A48" s="46"/>
+      <c r="B48" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="83" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="107"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108"/>
+      <c r="G48" s="108"/>
+      <c r="H48" s="108"/>
+      <c r="I48" s="23"/>
+    </row>
+    <row r="49" spans="1:9" s="24" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A49" s="46"/>
+      <c r="B49" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="130"/>
+      <c r="E49" s="131"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="131"/>
+      <c r="I49" s="23"/>
+    </row>
+    <row r="50" spans="1:9" s="24" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A50" s="46"/>
+      <c r="B50" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="83" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="130"/>
+      <c r="E50" s="131"/>
+      <c r="F50" s="131"/>
+      <c r="G50" s="131"/>
+      <c r="H50" s="131"/>
+      <c r="I50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" s="26" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A51" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="58"/>
+      <c r="C51" s="84" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="132"/>
+      <c r="E51" s="132"/>
+      <c r="F51" s="132"/>
+      <c r="G51" s="132"/>
+      <c r="H51" s="132"/>
+      <c r="I51" s="25"/>
+    </row>
+    <row r="52" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A52" s="48"/>
+      <c r="B52" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="85" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="133"/>
+      <c r="E52" s="134"/>
+      <c r="F52" s="134"/>
+      <c r="G52" s="134"/>
+      <c r="H52" s="134"/>
+      <c r="I52" s="27"/>
+    </row>
+    <row r="53" spans="1:9" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A53" s="48"/>
+      <c r="B53" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="112" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A7" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="113" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A8" s="62"/>
-      <c r="B8" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="62"/>
-      <c r="B9" s="83" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A10" s="62"/>
-      <c r="B10" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="114" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A11" s="62"/>
-      <c r="B11" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="114" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="62"/>
-      <c r="B12" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="114" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A13" s="62"/>
-      <c r="B13" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="114" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="62"/>
-      <c r="B14" s="83" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="114" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="95"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="62"/>
-      <c r="B15" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A16" s="62"/>
-      <c r="B16" s="83" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="114" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="62"/>
-      <c r="B17" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="114"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="62"/>
-      <c r="B18" s="83" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="114"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A19" s="62"/>
-      <c r="B19" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="114"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="62"/>
-      <c r="B20" s="83" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="114"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="62"/>
-      <c r="B21" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="114"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="127" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="115" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="63"/>
-      <c r="B23" s="133" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="97"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
-    </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="63"/>
-      <c r="B24" s="133" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="116" t="s">
-        <v>117</v>
-      </c>
-      <c r="D24" s="98"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="63"/>
-      <c r="B25" s="133" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="99"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="63"/>
-      <c r="B26" s="133" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="116" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="99"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A27" s="63"/>
-      <c r="B27" s="133" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="116" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="99"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A28" s="63"/>
-      <c r="B28" s="133" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="99"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="18"/>
-    </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A29" s="63"/>
-      <c r="B29" s="133" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="116" t="s">
-        <v>122</v>
-      </c>
-      <c r="D29" s="99"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A30" s="63"/>
-      <c r="B30" s="133" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="116" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="97"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A31" s="63"/>
-      <c r="B31" s="133" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="116" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="100"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="18"/>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="63"/>
-      <c r="B32" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="116" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="100"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="18"/>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A33" s="63"/>
-      <c r="B33" s="86" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="116" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="101"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="18"/>
-    </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="63"/>
-      <c r="B34" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="116" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="100"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="18"/>
-    </row>
-    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="64"/>
-      <c r="B35" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="116" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="99"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="25"/>
-    </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A36" s="63"/>
-      <c r="B36" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="100"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="18"/>
-    </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A37" s="63"/>
-      <c r="B37" s="86" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="116" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="100"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="18"/>
-    </row>
-    <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="128" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="117" t="s">
-        <v>146</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-    </row>
-    <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="65"/>
-      <c r="B39" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="118" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="102"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="30"/>
-    </row>
-    <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="65"/>
-      <c r="B40" s="88" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" s="102"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="30"/>
-    </row>
-    <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A41" s="65"/>
-      <c r="B41" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="118" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="102"/>
-      <c r="E41" s="102"/>
-      <c r="F41" s="102"/>
-      <c r="G41" s="102"/>
-      <c r="H41" s="102"/>
-      <c r="I41" s="30"/>
-    </row>
-    <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A42" s="65"/>
-      <c r="B42" s="130" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="118" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="102"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="30"/>
-    </row>
-    <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A43" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="78"/>
-      <c r="C43" s="119" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="103"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="34"/>
-    </row>
-    <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A44" s="67"/>
-      <c r="B44" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="120" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="104"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
-    </row>
-    <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A45" s="67"/>
-      <c r="B45" s="89" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="120" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="105"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="37"/>
-    </row>
-    <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A46" s="67"/>
-      <c r="B46" s="89" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="120" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="106"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="37"/>
-    </row>
-    <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A47" s="67"/>
-      <c r="B47" s="89" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="107"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="37"/>
-    </row>
-    <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
-      <c r="A48" s="67"/>
-      <c r="B48" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="120" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="105"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="37"/>
-    </row>
-    <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A49" s="67"/>
-      <c r="B49" s="89" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="120" t="s">
-        <v>143</v>
-      </c>
-      <c r="D49" s="106"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="37"/>
-    </row>
-    <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A50" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="79"/>
-      <c r="C50" s="121" t="s">
+      <c r="C53" s="85" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="133"/>
+      <c r="E53" s="134"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="134"/>
+      <c r="H53" s="134"/>
+      <c r="I53" s="27"/>
+    </row>
+    <row r="54" spans="1:9" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.5">
+      <c r="A54" s="92" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" s="59"/>
+      <c r="C54" s="86" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" s="135"/>
+      <c r="E54" s="135"/>
+      <c r="F54" s="135"/>
+      <c r="G54" s="135"/>
+      <c r="H54" s="135"/>
+      <c r="I54" s="29"/>
+    </row>
+    <row r="55" spans="1:9" s="32" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A55" s="49"/>
+      <c r="B55" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="87" t="s">
         <v>148</v>
       </c>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-    </row>
-    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="69"/>
-      <c r="B51" s="90" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="122" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="108"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="45"/>
-    </row>
-    <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A52" s="69"/>
-      <c r="B52" s="90" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="122" t="s">
-        <v>145</v>
-      </c>
-      <c r="D52" s="108"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="45"/>
-    </row>
-    <row r="53" spans="1:9" s="48" customFormat="1" ht="42" x14ac:dyDescent="0.5">
-      <c r="A53" s="129" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="80"/>
-      <c r="C53" s="123" t="s">
+      <c r="D55" s="136"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="137"/>
+      <c r="G55" s="137"/>
+      <c r="H55" s="137"/>
+      <c r="I55" s="31"/>
+    </row>
+    <row r="56" spans="1:9" s="32" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A56" s="49"/>
+      <c r="B56" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="87" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
-    </row>
-    <row r="54" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A54" s="70"/>
-      <c r="B54" s="91" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="124" t="s">
+      <c r="D56" s="136"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="137"/>
+      <c r="G56" s="137"/>
+      <c r="H56" s="137"/>
+      <c r="I56" s="31"/>
+    </row>
+    <row r="57" spans="1:9" s="32" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A57" s="49"/>
+      <c r="B57" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="D54" s="109"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="50"/>
-    </row>
-    <row r="55" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A55" s="70"/>
-      <c r="B55" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="124" t="s">
+      <c r="D57" s="136"/>
+      <c r="E57" s="137"/>
+      <c r="F57" s="137"/>
+      <c r="G57" s="137"/>
+      <c r="H57" s="137"/>
+      <c r="I57" s="31"/>
+    </row>
+    <row r="58" spans="1:9" s="32" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A58" s="49"/>
+      <c r="B58" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="87" t="s">
         <v>151</v>
       </c>
-      <c r="D55" s="109"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="50"/>
-    </row>
-    <row r="56" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A56" s="70"/>
-      <c r="B56" s="91" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="124" t="s">
+      <c r="D58" s="136"/>
+      <c r="E58" s="137"/>
+      <c r="F58" s="137"/>
+      <c r="G58" s="137"/>
+      <c r="H58" s="137"/>
+      <c r="I58" s="31"/>
+    </row>
+    <row r="59" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A59" s="49"/>
+      <c r="B59" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="87"/>
+      <c r="D59" s="136"/>
+      <c r="E59" s="137"/>
+      <c r="F59" s="137"/>
+      <c r="G59" s="137"/>
+      <c r="H59" s="137"/>
+      <c r="I59" s="31"/>
+    </row>
+    <row r="60" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A60" s="49"/>
+      <c r="B60" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="87"/>
+      <c r="D60" s="136"/>
+      <c r="E60" s="137"/>
+      <c r="F60" s="137"/>
+      <c r="G60" s="137"/>
+      <c r="H60" s="137"/>
+      <c r="I60" s="31"/>
+    </row>
+    <row r="61" spans="1:9" s="32" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A61" s="49"/>
+      <c r="B61" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="87"/>
+      <c r="D61" s="136"/>
+      <c r="E61" s="137"/>
+      <c r="F61" s="137"/>
+      <c r="G61" s="137"/>
+      <c r="H61" s="137"/>
+      <c r="I61" s="31"/>
+    </row>
+    <row r="62" spans="1:9" s="32" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A62" s="49"/>
+      <c r="B62" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="87"/>
+      <c r="D62" s="136"/>
+      <c r="E62" s="137"/>
+      <c r="F62" s="137"/>
+      <c r="G62" s="137"/>
+      <c r="H62" s="137"/>
+      <c r="I62" s="31"/>
+    </row>
+    <row r="63" spans="1:9" s="34" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A63" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="60"/>
+      <c r="C63" s="88" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" s="138"/>
+      <c r="E63" s="138"/>
+      <c r="F63" s="138"/>
+      <c r="G63" s="138"/>
+      <c r="H63" s="138"/>
+      <c r="I63" s="33"/>
+    </row>
+    <row r="64" spans="1:9" s="36" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A64" s="51"/>
+      <c r="B64" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="109"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="50"/>
-    </row>
-    <row r="57" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A57" s="70"/>
-      <c r="B57" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="C57" s="124" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" s="109"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="50"/>
-    </row>
-    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="70"/>
-      <c r="B58" s="91" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="124"/>
-      <c r="D58" s="109"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="50"/>
-    </row>
-    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="70"/>
-      <c r="B59" s="91" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="124"/>
-      <c r="D59" s="109"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="50"/>
-    </row>
-    <row r="60" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A60" s="70"/>
-      <c r="B60" s="93" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="124"/>
-      <c r="D60" s="109"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="50"/>
-    </row>
-    <row r="61" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A61" s="70"/>
-      <c r="B61" s="93" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="124"/>
-      <c r="D61" s="109"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="50"/>
-    </row>
-    <row r="62" spans="1:9" s="53" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A62" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" s="81"/>
-      <c r="C62" s="125" t="s">
-        <v>154</v>
-      </c>
-      <c r="D62" s="52"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-    </row>
-    <row r="63" spans="1:9" s="56" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A63" s="72"/>
-      <c r="B63" s="94" t="s">
+      <c r="D64" s="139"/>
+      <c r="E64" s="140"/>
+      <c r="F64" s="140"/>
+      <c r="G64" s="140"/>
+      <c r="H64" s="140"/>
+      <c r="I64" s="35"/>
+    </row>
+    <row r="65" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A65" s="51"/>
+      <c r="B65" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="126" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" s="110"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="55"/>
-    </row>
-    <row r="64" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="72"/>
-      <c r="B64" s="94" t="s">
-        <v>98</v>
-      </c>
-      <c r="C64" s="126" t="s">
-        <v>166</v>
-      </c>
-      <c r="D64" s="110"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="55"/>
+      <c r="C65" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="D65" s="139"/>
+      <c r="E65" s="140"/>
+      <c r="F65" s="140"/>
+      <c r="G65" s="140"/>
+      <c r="H65" s="140"/>
+      <c r="I65" s="35"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2737,13 +2785,13 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$J$2:$J$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D49:H49</xm:sqref>
+          <xm:sqref>D50:H50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{093E1169-867D-4A32-AC3C-DC58C26E3C39}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D64:H64</xm:sqref>
+          <xm:sqref>D65:H65</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
@@ -2751,17 +2799,17 @@
           </x14:formula1>
           <xm:sqref>E9:H9</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
+          <x14:formula1>
+            <xm:f>'Drop Down List Values'!$L$2:$L$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D41:H41</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38BD6F45-E1D6-4C47-97BB-112AE837004E}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!K2:K4</xm:f>
           </x14:formula1>
           <xm:sqref>D46:H46</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$L$2:$L$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>D41:H41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2773,7 +2821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8BFBD-18C1-4ED5-A02E-9841686C259E}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2811,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
         <v>44</v>
@@ -2823,16 +2871,16 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2849,31 +2897,31 @@
         <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -2881,7 +2929,7 @@
         <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -2890,36 +2938,36 @@
         <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -2931,31 +2979,31 @@
         <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
         <v>53</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2972,22 +3020,22 @@
         <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
         <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2998,16 +3046,16 @@
         <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -3015,13 +3063,13 @@
         <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3230,6 +3278,29 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
+      <Description>YVWEJ5DVYS2U-421999773-68</Description>
+    </_dlc_DocIdUrl>
+    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -3279,29 +3350,6 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
-      <Description>YVWEJ5DVYS2U-421999773-68</Description>
-    </_dlc_DocIdUrl>
-    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
@@ -3323,9 +3371,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3339,19 +3397,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated raven MDI-To-EDRS spreadsheet with better language.
</commit_message>
<xml_diff>
--- a/MDI_Raven_Excel_Schema.xlsx
+++ b/MDI_Raven_Excel_Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-iasa-sandbox\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC6BFF82-2DF5-42E0-82F3-1BC2B8397114}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA2C7362-6C12-4871-A147-5B41DDF86618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="MDI RAVEN Input Schema" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Location of death</t>
   </si>
   <si>
-    <t>Jurisdiction</t>
-  </si>
-  <si>
     <t>Place of death</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>Asked But Unknown</t>
   </si>
   <si>
-    <t>Chief Medical Examiner/Coroner</t>
-  </si>
-  <si>
     <t>Natural death</t>
   </si>
   <si>
@@ -314,9 +308,6 @@
   </si>
   <si>
     <t>End of Cases</t>
-  </si>
-  <si>
-    <t>Certifier</t>
   </si>
   <si>
     <t>Certifier Name</t>
@@ -559,9 +550,6 @@
   </si>
   <si>
     <t>Primary Address of the medical examiner's office or primary address. Multiple lines are supported.</t>
-  </si>
-  <si>
-    <t>This section describes the certifier of the case, if the case has been certified. Oftentimes, the Chief Medical Examiner and the Certifier can be the same party. If the case is not certified, leave blank</t>
   </si>
   <si>
     <t xml:space="preserve">Name of the Certifier.
@@ -665,6 +653,12 @@
   </si>
   <si>
     <t>INVALID</t>
+  </si>
+  <si>
+    <t>Death Pronouncement</t>
+  </si>
+  <si>
+    <t>Death Certifier</t>
   </si>
 </sst>
 </file>
@@ -747,7 +741,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -850,18 +844,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC9C9C9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1C67F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5D5A1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,7 +953,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1159,24 +1141,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1193,13 +1157,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -1212,7 +1173,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1249,9 +1209,6 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1312,10 +1269,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1359,12 +1312,6 @@
     <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1390,6 +1337,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1404,9 +1354,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC9C9C9"/>
       <color rgb="FFF5D5A1"/>
       <color rgb="FFF1C67F"/>
-      <color rgb="FFC9C9C9"/>
       <color rgb="FF9F9F9F"/>
       <color rgb="FFFFB9AB"/>
       <color rgb="FFFF856D"/>
@@ -1728,74 +1678,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="58" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="73" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="82" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="53" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="73" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="82" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="134" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="135" t="s">
-        <v>174</v>
+      <c r="A3" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="121" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="122" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="111" t="s">
-        <v>104</v>
+      <c r="B4" s="66"/>
+      <c r="C4" s="100" t="s">
+        <v>101</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1805,42 +1755,42 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A5" s="60"/>
-      <c r="B5" s="131" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="112" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="118" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A6" s="55"/>
+      <c r="B6" s="119" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="101" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A7" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="102" t="s">
         <v>105</v>
-      </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="60"/>
-      <c r="B6" s="132" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="112" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A7" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="113" t="s">
-        <v>108</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1850,12 +1800,12 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A8" s="62"/>
-      <c r="B8" s="83" t="s">
+      <c r="A8" s="57"/>
+      <c r="B8" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="114" t="s">
-        <v>107</v>
+      <c r="C8" s="103" t="s">
+        <v>104</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="9"/>
@@ -1865,12 +1815,12 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="62"/>
-      <c r="B9" s="83" t="s">
+      <c r="A9" s="57"/>
+      <c r="B9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="114" t="s">
-        <v>111</v>
+      <c r="C9" s="103" t="s">
+        <v>108</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="9"/>
@@ -1880,12 +1830,12 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A10" s="62"/>
-      <c r="B10" s="83" t="s">
+      <c r="A10" s="57"/>
+      <c r="B10" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="114" t="s">
-        <v>110</v>
+      <c r="C10" s="103" t="s">
+        <v>107</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="9"/>
@@ -1895,12 +1845,12 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A11" s="62"/>
-      <c r="B11" s="84" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="114" t="s">
-        <v>109</v>
+      <c r="A11" s="57"/>
+      <c r="B11" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="103" t="s">
+        <v>106</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="9"/>
@@ -1910,12 +1860,12 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="62"/>
-      <c r="B12" s="83" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="114" t="s">
-        <v>159</v>
+      <c r="C12" s="103" t="s">
+        <v>155</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="9"/>
@@ -1925,12 +1875,12 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A13" s="62"/>
-      <c r="B13" s="83" t="s">
+      <c r="A13" s="57"/>
+      <c r="B13" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="114" t="s">
-        <v>112</v>
+      <c r="C13" s="103" t="s">
+        <v>109</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="9"/>
@@ -1940,14 +1890,14 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="62"/>
-      <c r="B14" s="83" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="114" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="95"/>
+      <c r="C14" s="103" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="85"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -1955,11 +1905,11 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="62"/>
-      <c r="B15" s="83" t="s">
+      <c r="A15" s="57"/>
+      <c r="B15" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="114"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="14"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1968,14 +1918,14 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A16" s="62"/>
-      <c r="B16" s="83" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="114" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="96"/>
+      <c r="C16" s="103" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="86"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1983,11 +1933,11 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="62"/>
-      <c r="B17" s="83" t="s">
+      <c r="A17" s="57"/>
+      <c r="B17" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="114"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="14"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1996,11 +1946,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="62"/>
-      <c r="B18" s="83" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="114"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="103"/>
       <c r="D18" s="14"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -2009,11 +1959,11 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A19" s="62"/>
-      <c r="B19" s="85" t="s">
+      <c r="A19" s="57"/>
+      <c r="B19" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="114"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="14"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -2022,11 +1972,11 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="62"/>
-      <c r="B20" s="83" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="114"/>
+      <c r="C20" s="103"/>
       <c r="D20" s="14"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -2035,11 +1985,11 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="62"/>
-      <c r="B21" s="83" t="s">
+      <c r="A21" s="57"/>
+      <c r="B21" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="114"/>
+      <c r="C21" s="103"/>
       <c r="D21" s="14"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -2048,12 +1998,12 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="127" t="s">
+      <c r="A22" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="115" t="s">
-        <v>115</v>
+      <c r="B22" s="68"/>
+      <c r="C22" s="104" t="s">
+        <v>112</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -2063,14 +2013,14 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="63"/>
-      <c r="B23" s="133" t="s">
+      <c r="A23" s="58"/>
+      <c r="B23" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="97"/>
+      <c r="C23" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="87"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2078,14 +2028,14 @@
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="63"/>
-      <c r="B24" s="133" t="s">
+      <c r="A24" s="58"/>
+      <c r="B24" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="116" t="s">
-        <v>117</v>
-      </c>
-      <c r="D24" s="98"/>
+      <c r="C24" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="88"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -2093,14 +2043,14 @@
       <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="63"/>
-      <c r="B25" s="133" t="s">
+      <c r="A25" s="58"/>
+      <c r="B25" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="99"/>
+      <c r="C25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="89"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -2108,14 +2058,14 @@
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="63"/>
-      <c r="B26" s="133" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="116" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="99"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="120" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="89"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -2123,14 +2073,14 @@
       <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A27" s="63"/>
-      <c r="B27" s="133" t="s">
+      <c r="A27" s="58"/>
+      <c r="B27" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="116" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="99"/>
+      <c r="C27" s="105" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="89"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -2138,14 +2088,14 @@
       <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A28" s="63"/>
-      <c r="B28" s="133" t="s">
+      <c r="A28" s="58"/>
+      <c r="B28" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="99"/>
+      <c r="C28" s="105" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="89"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -2153,14 +2103,14 @@
       <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A29" s="63"/>
-      <c r="B29" s="133" t="s">
+      <c r="A29" s="58"/>
+      <c r="B29" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="116" t="s">
-        <v>122</v>
-      </c>
-      <c r="D29" s="99"/>
+      <c r="C29" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="89"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -2168,14 +2118,14 @@
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A30" s="63"/>
-      <c r="B30" s="133" t="s">
+      <c r="A30" s="58"/>
+      <c r="B30" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="116" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="97"/>
+      <c r="C30" s="105" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="87"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
@@ -2183,14 +2133,14 @@
       <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A31" s="63"/>
-      <c r="B31" s="133" t="s">
+      <c r="A31" s="58"/>
+      <c r="B31" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="116" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="100"/>
+      <c r="C31" s="105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="90"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -2198,14 +2148,14 @@
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="63"/>
-      <c r="B32" s="86" t="s">
+      <c r="A32" s="58"/>
+      <c r="B32" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="116" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="100"/>
+      <c r="C32" s="105" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="90"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -2213,14 +2163,14 @@
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A33" s="63"/>
-      <c r="B33" s="86" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="116" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="101"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="91"/>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
@@ -2228,14 +2178,14 @@
       <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="63"/>
-      <c r="B34" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="116" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="100"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="105" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="90"/>
       <c r="E34" s="22"/>
       <c r="F34" s="24"/>
       <c r="G34" s="22"/>
@@ -2243,14 +2193,14 @@
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="64"/>
-      <c r="B35" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="116" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="99"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="105" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="89"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -2258,14 +2208,14 @@
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A36" s="63"/>
-      <c r="B36" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="100"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="105" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="90"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -2273,14 +2223,14 @@
       <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A37" s="63"/>
-      <c r="B37" s="86" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="116" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="100"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="105" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="90"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -2288,12 +2238,12 @@
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="128" t="s">
+      <c r="A38" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="117" t="s">
-        <v>146</v>
+      <c r="B38" s="69"/>
+      <c r="C38" s="106" t="s">
+        <v>143</v>
       </c>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
@@ -2303,14 +2253,14 @@
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="65"/>
-      <c r="B39" s="87" t="s">
+      <c r="A39" s="60"/>
+      <c r="B39" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="118" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="102"/>
+      <c r="C39" s="107" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="92"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
@@ -2318,14 +2268,14 @@
       <c r="I39" s="30"/>
     </row>
     <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="65"/>
-      <c r="B40" s="88" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" s="102"/>
+      <c r="A40" s="60"/>
+      <c r="B40" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="107" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="92"/>
       <c r="E40" s="29"/>
       <c r="F40" s="32"/>
       <c r="G40" s="29"/>
@@ -2333,29 +2283,29 @@
       <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A41" s="65"/>
-      <c r="B41" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="118" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="102"/>
-      <c r="E41" s="102"/>
-      <c r="F41" s="102"/>
-      <c r="G41" s="102"/>
-      <c r="H41" s="102"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="92"/>
+      <c r="H41" s="92"/>
       <c r="I41" s="30"/>
     </row>
     <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A42" s="65"/>
-      <c r="B42" s="130" t="s">
+      <c r="A42" s="60"/>
+      <c r="B42" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="118" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="102"/>
+      <c r="C42" s="107" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="92"/>
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
@@ -2363,14 +2313,14 @@
       <c r="I42" s="30"/>
     </row>
     <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A43" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="78"/>
-      <c r="C43" s="119" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="103"/>
+      <c r="A43" s="123" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="70"/>
+      <c r="C43" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="93"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
@@ -2378,14 +2328,14 @@
       <c r="I43" s="34"/>
     </row>
     <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A44" s="67"/>
-      <c r="B44" s="89" t="s">
+      <c r="A44" s="61"/>
+      <c r="B44" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="120" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="104"/>
+      <c r="C44" s="109" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="94"/>
       <c r="E44" s="36"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
@@ -2393,14 +2343,14 @@
       <c r="I44" s="37"/>
     </row>
     <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A45" s="67"/>
-      <c r="B45" s="89" t="s">
+      <c r="A45" s="61"/>
+      <c r="B45" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="120" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="105"/>
+      <c r="C45" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="95"/>
       <c r="E45" s="39"/>
       <c r="F45" s="39"/>
       <c r="G45" s="39"/>
@@ -2408,14 +2358,14 @@
       <c r="I45" s="37"/>
     </row>
     <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A46" s="67"/>
-      <c r="B46" s="89" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="120" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46" s="106"/>
+      <c r="A46" s="61"/>
+      <c r="B46" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="96"/>
       <c r="E46" s="40"/>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
@@ -2423,14 +2373,14 @@
       <c r="I46" s="37"/>
     </row>
     <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A47" s="67"/>
-      <c r="B47" s="89" t="s">
+      <c r="A47" s="61"/>
+      <c r="B47" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="107"/>
+      <c r="C47" s="109" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="97"/>
       <c r="E47" s="41"/>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
@@ -2438,14 +2388,14 @@
       <c r="I47" s="37"/>
     </row>
     <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
-      <c r="A48" s="67"/>
-      <c r="B48" s="89" t="s">
+      <c r="A48" s="61"/>
+      <c r="B48" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="120" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="105"/>
+      <c r="C48" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="95"/>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
       <c r="G48" s="39"/>
@@ -2453,14 +2403,14 @@
       <c r="I48" s="37"/>
     </row>
     <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A49" s="67"/>
-      <c r="B49" s="89" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="120" t="s">
-        <v>143</v>
-      </c>
-      <c r="D49" s="106"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="109" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="96"/>
       <c r="E49" s="40"/>
       <c r="F49" s="40"/>
       <c r="G49" s="40"/>
@@ -2468,12 +2418,12 @@
       <c r="I49" s="37"/>
     </row>
     <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A50" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="79"/>
-      <c r="C50" s="121" t="s">
-        <v>148</v>
+      <c r="A50" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="71"/>
+      <c r="C50" s="110" t="s">
+        <v>145</v>
       </c>
       <c r="D50" s="42"/>
       <c r="E50" s="42"/>
@@ -2483,14 +2433,14 @@
       <c r="I50" s="42"/>
     </row>
     <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="69"/>
-      <c r="B51" s="90" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="122" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="108"/>
+      <c r="A51" s="63"/>
+      <c r="B51" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="111" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" s="98"/>
       <c r="E51" s="44"/>
       <c r="F51" s="44"/>
       <c r="G51" s="44"/>
@@ -2498,27 +2448,27 @@
       <c r="I51" s="45"/>
     </row>
     <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A52" s="69"/>
-      <c r="B52" s="90" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="122" t="s">
-        <v>145</v>
-      </c>
-      <c r="D52" s="108"/>
+      <c r="A52" s="63"/>
+      <c r="B52" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="111" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="98"/>
       <c r="E52" s="44"/>
       <c r="F52" s="44"/>
       <c r="G52" s="44"/>
       <c r="H52" s="44"/>
       <c r="I52" s="45"/>
     </row>
-    <row r="53" spans="1:9" s="48" customFormat="1" ht="42" x14ac:dyDescent="0.5">
-      <c r="A53" s="129" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="80"/>
-      <c r="C53" s="123" t="s">
-        <v>149</v>
+    <row r="53" spans="1:9" s="48" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A53" s="116" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="72"/>
+      <c r="C53" s="112" t="s">
+        <v>146</v>
       </c>
       <c r="D53" s="47"/>
       <c r="E53" s="47"/>
@@ -2528,14 +2478,14 @@
       <c r="I53" s="47"/>
     </row>
     <row r="54" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A54" s="70"/>
-      <c r="B54" s="91" t="s">
+      <c r="A54" s="64"/>
+      <c r="B54" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="124" t="s">
-        <v>150</v>
-      </c>
-      <c r="D54" s="109"/>
+      <c r="C54" s="113" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="99"/>
       <c r="E54" s="49"/>
       <c r="F54" s="49"/>
       <c r="G54" s="49"/>
@@ -2543,14 +2493,14 @@
       <c r="I54" s="50"/>
     </row>
     <row r="55" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A55" s="70"/>
-      <c r="B55" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="124" t="s">
-        <v>151</v>
-      </c>
-      <c r="D55" s="109"/>
+      <c r="A55" s="64"/>
+      <c r="B55" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="113" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="99"/>
       <c r="E55" s="49"/>
       <c r="F55" s="49"/>
       <c r="G55" s="49"/>
@@ -2558,14 +2508,14 @@
       <c r="I55" s="50"/>
     </row>
     <row r="56" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A56" s="70"/>
-      <c r="B56" s="91" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="124" t="s">
-        <v>152</v>
-      </c>
-      <c r="D56" s="109"/>
+      <c r="A56" s="64"/>
+      <c r="B56" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="113" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="99"/>
       <c r="E56" s="49"/>
       <c r="F56" s="49"/>
       <c r="G56" s="49"/>
@@ -2573,14 +2523,14 @@
       <c r="I56" s="50"/>
     </row>
     <row r="57" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A57" s="70"/>
-      <c r="B57" s="91" t="s">
+      <c r="A57" s="64"/>
+      <c r="B57" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="C57" s="124" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" s="109"/>
+      <c r="C57" s="113" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" s="99"/>
       <c r="E57" s="49"/>
       <c r="F57" s="49"/>
       <c r="G57" s="49"/>
@@ -2588,12 +2538,12 @@
       <c r="I57" s="50"/>
     </row>
     <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="70"/>
-      <c r="B58" s="91" t="s">
+      <c r="A58" s="64"/>
+      <c r="B58" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="124"/>
-      <c r="D58" s="109"/>
+      <c r="C58" s="113"/>
+      <c r="D58" s="99"/>
       <c r="E58" s="49"/>
       <c r="F58" s="49"/>
       <c r="G58" s="49"/>
@@ -2601,12 +2551,12 @@
       <c r="I58" s="50"/>
     </row>
     <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="70"/>
-      <c r="B59" s="91" t="s">
+      <c r="A59" s="64"/>
+      <c r="B59" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="124"/>
-      <c r="D59" s="109"/>
+      <c r="C59" s="113"/>
+      <c r="D59" s="99"/>
       <c r="E59" s="49"/>
       <c r="F59" s="49"/>
       <c r="G59" s="49"/>
@@ -2614,12 +2564,12 @@
       <c r="I59" s="50"/>
     </row>
     <row r="60" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A60" s="70"/>
-      <c r="B60" s="93" t="s">
+      <c r="A60" s="64"/>
+      <c r="B60" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="124"/>
-      <c r="D60" s="109"/>
+      <c r="C60" s="113"/>
+      <c r="D60" s="99"/>
       <c r="E60" s="49"/>
       <c r="F60" s="49"/>
       <c r="G60" s="49"/>
@@ -2627,62 +2577,47 @@
       <c r="I60" s="50"/>
     </row>
     <row r="61" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A61" s="70"/>
-      <c r="B61" s="93" t="s">
+      <c r="A61" s="64"/>
+      <c r="B61" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="124"/>
-      <c r="D61" s="109"/>
+      <c r="C61" s="113"/>
+      <c r="D61" s="99"/>
       <c r="E61" s="49"/>
       <c r="F61" s="49"/>
       <c r="G61" s="49"/>
       <c r="H61" s="49"/>
       <c r="I61" s="50"/>
     </row>
-    <row r="62" spans="1:9" s="53" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A62" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="B62" s="81"/>
-      <c r="C62" s="125" t="s">
-        <v>154</v>
-      </c>
-      <c r="D62" s="52"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="52"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-    </row>
-    <row r="63" spans="1:9" s="56" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A63" s="72"/>
-      <c r="B63" s="94" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="126" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" s="110"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="55"/>
-    </row>
-    <row r="64" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="72"/>
-      <c r="B64" s="94" t="s">
-        <v>98</v>
-      </c>
-      <c r="C64" s="126" t="s">
-        <v>166</v>
-      </c>
-      <c r="D64" s="110"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="55"/>
+    <row r="62" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A62" s="64"/>
+      <c r="B62" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="113" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="99"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="50"/>
+    </row>
+    <row r="63" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A63" s="64"/>
+      <c r="B63" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="113" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" s="99"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="50"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2743,7 +2678,7 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D64:H64</xm:sqref>
+          <xm:sqref>D63:H63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
@@ -2751,17 +2686,17 @@
           </x14:formula1>
           <xm:sqref>E9:H9</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
+          <x14:formula1>
+            <xm:f>'Drop Down List Values'!$L$2:$L$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D41:H41</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38BD6F45-E1D6-4C47-97BB-112AE837004E}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!K2:K4</xm:f>
           </x14:formula1>
           <xm:sqref>D46:H46</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$L$2:$L$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>D41:H41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2802,19 +2737,19 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
         <v>25</v>
@@ -2823,205 +2758,205 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="M4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3031,6 +2966,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -3229,65 +3223,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3303,6 +3238,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3322,36 +3273,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>